<commit_message>
EBEGU-1545 - Der Code vom Task EBEGU-1552 wurde teilweise entfernt, da das richtige Gesuch zu holen sehr langsam ist. Aus diesem Grund lassen wir in diesem Task lediglich den Teil von ExcelMerger. - Ab jetzt gibt es nur GesuchstellerKinderBetreuungExcelConverter. Die Reports von Kinder und Gesuchsteller verwenden diesen Converter und holen nur die Daten die sie brauchen - Kinder, Gesuchsteller und GesuchstellerKinderBetreuung funktionieren nun mit SXSSFSheet -> performance verbessern
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gesuchsteller.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\reporting\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="606"/>
+    <workbookView xWindow="975" yWindow="360" windowWidth="16380" windowHeight="8190" tabRatio="606"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -288,11 +293,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -475,15 +480,34 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -493,25 +517,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -586,13 +591,21 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -630,9 +643,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -664,9 +677,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -698,9 +712,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -873,17 +888,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL11"/>
+  <dimension ref="A1:AX9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.7109375"/>
     <col min="3" max="3" width="15.7109375" style="1"/>
@@ -906,7 +921,7 @@
     <col min="50" max="1003" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="21">
+    <row r="1" spans="1:50" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -916,10 +931,10 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -929,7 +944,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -938,109 +953,109 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="6" spans="1:50" s="7" customFormat="1">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:50" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="20" t="s">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="X6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="20"/>
-      <c r="AA6" s="20"/>
-      <c r="AB6" s="20"/>
-      <c r="AC6" s="20"/>
-      <c r="AD6" s="20"/>
-      <c r="AE6" s="20"/>
-      <c r="AF6" s="29"/>
-      <c r="AG6" s="29"/>
-      <c r="AH6" s="29"/>
-      <c r="AI6" s="29"/>
-      <c r="AJ6" s="29"/>
-      <c r="AK6" s="29"/>
-      <c r="AL6" s="29"/>
-      <c r="AM6" s="22" t="s">
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="24"/>
+      <c r="AI6" s="24"/>
+      <c r="AJ6" s="24"/>
+      <c r="AK6" s="24"/>
+      <c r="AL6" s="24"/>
+      <c r="AM6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="AN6" s="22"/>
-      <c r="AO6" s="22"/>
-      <c r="AP6" s="22" t="s">
+      <c r="AN6" s="25"/>
+      <c r="AO6" s="25"/>
+      <c r="AP6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="AQ6" s="22"/>
-      <c r="AR6" s="22"/>
-      <c r="AS6" s="22"/>
-      <c r="AT6" s="22"/>
-      <c r="AU6" s="22" t="s">
+      <c r="AQ6" s="25"/>
+      <c r="AR6" s="25"/>
+      <c r="AS6" s="25"/>
+      <c r="AT6" s="25"/>
+      <c r="AU6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="AV6" s="20" t="s">
+      <c r="AV6" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:50">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="20" t="s">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="23" t="s">
         <v>21</v>
       </c>
       <c r="O7" s="26" t="s">
@@ -1055,28 +1070,28 @@
       <c r="T7" s="27"/>
       <c r="U7" s="27"/>
       <c r="V7" s="9"/>
-      <c r="W7" s="30" t="s">
+      <c r="W7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="X7" s="20" t="s">
+      <c r="X7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="Y7" s="20" t="s">
+      <c r="Y7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="Z7" s="20" t="s">
+      <c r="Z7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="AA7" s="20" t="s">
+      <c r="AA7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="AB7" s="20" t="s">
+      <c r="AB7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="AC7" s="20" t="s">
+      <c r="AC7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="20" t="s">
+      <c r="AD7" s="23" t="s">
         <v>21</v>
       </c>
       <c r="AE7" s="26" t="s">
@@ -1091,49 +1106,49 @@
       <c r="AJ7" s="27"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="9"/>
-      <c r="AM7" s="21" t="s">
+      <c r="AM7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AN7" s="24" t="s">
+      <c r="AN7" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="AO7" s="22" t="s">
+      <c r="AO7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="AP7" s="24" t="s">
+      <c r="AP7" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="AQ7" s="24" t="s">
+      <c r="AQ7" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="AR7" s="22" t="s">
+      <c r="AR7" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="AS7" s="23" t="s">
+      <c r="AS7" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="AT7" s="22" t="s">
+      <c r="AT7" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="AU7" s="22"/>
-      <c r="AV7" s="20"/>
+      <c r="AU7" s="25"/>
+      <c r="AV7" s="23"/>
     </row>
-    <row r="8" spans="1:50">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
       <c r="P8" s="12" t="s">
         <v>4</v>
       </c>
@@ -1155,15 +1170,15 @@
       <c r="V8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="20"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20"/>
-      <c r="AE8" s="20"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23"/>
+      <c r="AE8" s="23"/>
       <c r="AF8" s="12" t="s">
         <v>4</v>
       </c>
@@ -1185,18 +1200,18 @@
       <c r="AL8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AM8" s="22"/>
-      <c r="AN8" s="25"/>
-      <c r="AO8" s="22"/>
-      <c r="AP8" s="25"/>
-      <c r="AQ8" s="25"/>
-      <c r="AR8" s="22"/>
-      <c r="AS8" s="22"/>
-      <c r="AT8" s="22"/>
-      <c r="AU8" s="22"/>
-      <c r="AV8" s="20"/>
+      <c r="AM8" s="25"/>
+      <c r="AN8" s="32"/>
+      <c r="AO8" s="25"/>
+      <c r="AP8" s="32"/>
+      <c r="AQ8" s="32"/>
+      <c r="AR8" s="25"/>
+      <c r="AS8" s="25"/>
+      <c r="AT8" s="25"/>
+      <c r="AU8" s="25"/>
+      <c r="AV8" s="23"/>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>33</v>
       </c>
@@ -1343,31 +1358,32 @@
       <c r="AV9" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="AW9" s="32" t="s">
+      <c r="AW9" s="20" t="s">
         <v>79</v>
       </c>
       <c r="AX9" s="8"/>
-    </row>
-    <row r="10" spans="1:50">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10"/>
-    </row>
-    <row r="11" spans="1:50">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="AP6:AT6"/>
+    <mergeCell ref="AU6:AU8"/>
+    <mergeCell ref="AV6:AV8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AE7:AE8"/>
+    <mergeCell ref="AF7:AK7"/>
+    <mergeCell ref="AO7:AO8"/>
+    <mergeCell ref="AR7:AR8"/>
+    <mergeCell ref="AS7:AS8"/>
+    <mergeCell ref="AT7:AT8"/>
+    <mergeCell ref="AN7:AN8"/>
+    <mergeCell ref="AP7:AP8"/>
+    <mergeCell ref="AQ7:AQ8"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="G6:V6"/>
     <mergeCell ref="W6:AL6"/>
@@ -1383,26 +1399,12 @@
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="P7:U7"/>
     <mergeCell ref="W7:W8"/>
-    <mergeCell ref="AP6:AT6"/>
-    <mergeCell ref="AU6:AU8"/>
-    <mergeCell ref="AV6:AV8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AE7:AE8"/>
-    <mergeCell ref="AF7:AK7"/>
     <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AM7:AM8"/>
-    <mergeCell ref="AO7:AO8"/>
-    <mergeCell ref="AR7:AR8"/>
-    <mergeCell ref="AS7:AS8"/>
-    <mergeCell ref="AT7:AT8"/>
-    <mergeCell ref="AN7:AN8"/>
-    <mergeCell ref="AP7:AP8"/>
-    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>